<commit_message>
Results from LSTM with wind speed
</commit_message>
<xml_diff>
--- a/Summary_results_models.xlsx
+++ b/Summary_results_models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33637\Documents\12. Advanced time series\11. Exercises\2. Computer exercise 4\1. Analyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5A293D-4EFC-43BE-899C-DFFE59AD3757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1ACAB1-AB04-4BBA-9C9F-319865D6EF72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D602D6F8-97D8-4126-9415-78D7A3E6B22F}"/>
   </bookViews>
@@ -34,14 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>Model type</t>
   </si>
   <si>
-    <t>1h ahead CI</t>
-  </si>
-  <si>
     <t>2h ahead CI</t>
   </si>
   <si>
@@ -106,13 +103,40 @@
   </si>
   <si>
     <t>Considered inputs</t>
+  </si>
+  <si>
+    <t>±2.98</t>
+  </si>
+  <si>
+    <t>* CI: 95% confidence intervals in MW</t>
+  </si>
+  <si>
+    <t>1h ahead CI*</t>
+  </si>
+  <si>
+    <t>Ideas to improve LSTM:</t>
+  </si>
+  <si>
+    <t>Initialization of FFNN part</t>
+  </si>
+  <si>
+    <t>Batch normalization</t>
+  </si>
+  <si>
+    <t>Gradient clipping</t>
+  </si>
+  <si>
+    <t>±4.24</t>
+  </si>
+  <si>
+    <t>±4.93</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +146,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -149,9 +181,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,17 +499,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D2DA29C-414F-430C-8AF3-0679F0BCB5C1}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22.54296875" customWidth="1"/>
     <col min="2" max="2" width="36.81640625" customWidth="1"/>
-    <col min="3" max="6" width="14.26953125" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" customWidth="1"/>
+    <col min="4" max="6" width="14.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -484,108 +518,142 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Last update with TARSO model
</commit_message>
<xml_diff>
--- a/Summary_results_models.xlsx
+++ b/Summary_results_models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33637\Documents\12. Advanced time series\11. Exercises\2. Computer exercise 4\1. Analyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1ACAB1-AB04-4BBA-9C9F-319865D6EF72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84588D6-30C6-42B1-B62C-B5EA10BA3476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D602D6F8-97D8-4126-9415-78D7A3E6B22F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>Model type</t>
   </si>
@@ -130,6 +130,21 @@
   </si>
   <si>
     <t>±4.93</t>
+  </si>
+  <si>
+    <t>past p 1h</t>
+  </si>
+  <si>
+    <t>Persistent</t>
+  </si>
+  <si>
+    <t>±3.25</t>
+  </si>
+  <si>
+    <t>±4.88</t>
+  </si>
+  <si>
+    <t>±6.03</t>
   </si>
 </sst>
 </file>
@@ -499,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D2DA29C-414F-430C-8AF3-0679F0BCB5C1}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -566,36 +581,36 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -603,16 +618,16 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -620,7 +635,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -628,31 +652,39 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Results of LSTM with wind speed
</commit_message>
<xml_diff>
--- a/Summary_results_models.xlsx
+++ b/Summary_results_models.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33637\Documents\12. Advanced time series\11. Exercises\2. Computer exercise 4\1. Analyse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33637\Documents\12. Advanced time series\11. Exercises\4. Computer exercise 4\1. Analyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84588D6-30C6-42B1-B62C-B5EA10BA3476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51341C3-47F0-446B-A7A9-D44D1844CB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D602D6F8-97D8-4126-9415-78D7A3E6B22F}"/>
   </bookViews>
@@ -105,9 +105,6 @@
     <t>Considered inputs</t>
   </si>
   <si>
-    <t>±2.98</t>
-  </si>
-  <si>
     <t>* CI: 95% confidence intervals in MW</t>
   </si>
   <si>
@@ -126,12 +123,6 @@
     <t>Gradient clipping</t>
   </si>
   <si>
-    <t>±4.24</t>
-  </si>
-  <si>
-    <t>±4.93</t>
-  </si>
-  <si>
     <t>past p 1h</t>
   </si>
   <si>
@@ -145,6 +136,15 @@
   </si>
   <si>
     <t>±6.03</t>
+  </si>
+  <si>
+    <t>±2.96</t>
+  </si>
+  <si>
+    <t>±4.22</t>
+  </si>
+  <si>
+    <t>±4.91</t>
   </si>
 </sst>
 </file>
@@ -517,7 +517,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -536,7 +536,7 @@
         <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -581,19 +581,19 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
         <v>33</v>
-      </c>
-      <c r="B4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -638,13 +638,13 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -665,27 +665,27 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>